<commit_message>
🚀 Added render.yaml and API deployment setup
</commit_message>
<xml_diff>
--- a/assessments_data.xlsx
+++ b/assessments_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6e123d794a8f9d70/ドキュメント/VS code/PYTHON/SHL_Assessment_Recommender_Final/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{8E81F27A-77FA-48A2-A996-BCD551E5E16A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C8923F5-D4DE-4116-9FB3-69BBA8BE41B9}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{8E81F27A-77FA-48A2-A996-BCD551E5E16A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A38008E0-F09A-4F0D-9BF2-ABEDEE4675EC}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="156">
   <si>
     <t>Assessment Name</t>
   </si>
@@ -482,6 +482,12 @@
   </si>
   <si>
     <t>Programming &amp; Skills</t>
+  </si>
+  <si>
+    <t>Full Stack Development</t>
+  </si>
+  <si>
+    <t>MERN Stack</t>
   </si>
 </sst>
 </file>
@@ -864,8 +870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="74" workbookViewId="0">
-      <selection activeCell="F101" sqref="F101"/>
+    <sheetView tabSelected="1" zoomScale="74" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -920,7 +926,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>154</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>46</v>
@@ -960,7 +966,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>155</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>48</v>
@@ -2900,106 +2906,106 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="B18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="B20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="B21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="B22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="B23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="B24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="B25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="B26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="B27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="B28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="B29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="B30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="B31" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="B32" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="B33" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="B34" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="B35" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="B36" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="B37" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="B38" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="B39" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="B40" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="B41" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="B42" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="B43" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="B44" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="B45" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="B46" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="B47" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="B48" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="B49" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="B50" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="B51" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="B52" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="B53" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="B54" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="B55" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="B56" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="B57" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="B58" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="B59" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="B60" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="B61" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="B62" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="B63" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="B64" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="B65" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="B66" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="B67" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="B68" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="B69" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="B70" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="B71" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="B72" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="B73" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="B74" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="B75" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="B76" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="B77" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="B78" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="B79" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="B80" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="B81" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="B82" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
-    <hyperlink ref="B83" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="B84" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="B85" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
-    <hyperlink ref="B86" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
-    <hyperlink ref="B87" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="B88" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="B89" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="B90" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
-    <hyperlink ref="B91" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
-    <hyperlink ref="B92" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="B93" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="B94" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
-    <hyperlink ref="B95" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
-    <hyperlink ref="B96" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
-    <hyperlink ref="B97" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
-    <hyperlink ref="B98" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
-    <hyperlink ref="B99" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
-    <hyperlink ref="B100" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
-    <hyperlink ref="B101" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="B101" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="B100" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="B99" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="B98" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="B97" r:id="rId5" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="B96" r:id="rId6" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="B95" r:id="rId7" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="B94" r:id="rId8" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="B93" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="B92" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="B91" r:id="rId11" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="B90" r:id="rId12" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="B89" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="B88" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="B87" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="B86" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="B85" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="B84" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="B83" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="B82" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="B81" r:id="rId21" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="B80" r:id="rId22" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="B79" r:id="rId23" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="B78" r:id="rId24" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="B77" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="B76" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="B75" r:id="rId27" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="B74" r:id="rId28" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="B73" r:id="rId29" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="B72" r:id="rId30" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="B71" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="B70" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="B69" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="B68" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="B67" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="B66" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="B65" r:id="rId37" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="B64" r:id="rId38" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="B63" r:id="rId39" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="B62" r:id="rId40" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="B61" r:id="rId41" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="B60" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="B59" r:id="rId43" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="B58" r:id="rId44" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="B57" r:id="rId45" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="B56" r:id="rId46" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="B55" r:id="rId47" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="B54" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="B53" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="B52" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="B51" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="B50" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="B49" r:id="rId53" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="B48" r:id="rId54" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="B47" r:id="rId55" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="B46" r:id="rId56" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="B45" r:id="rId57" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="B44" r:id="rId58" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="B43" r:id="rId59" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="B42" r:id="rId60" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="B41" r:id="rId61" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="B40" r:id="rId62" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="B39" r:id="rId63" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="B38" r:id="rId64" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="B37" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="B36" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="B35" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="B34" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="B33" r:id="rId69" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="B32" r:id="rId70" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="B31" r:id="rId71" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="B30" r:id="rId72" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="B29" r:id="rId73" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="B28" r:id="rId74" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="B27" r:id="rId75" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="B26" r:id="rId76" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="B25" r:id="rId77" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="B24" r:id="rId78" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="B23" r:id="rId79" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="B22" r:id="rId80" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B21" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B20" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B19" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B18" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B17" r:id="rId85" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B16" r:id="rId86" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B15" r:id="rId87" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B14" r:id="rId88" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B13" r:id="rId89" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B12" r:id="rId90" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B11" r:id="rId91" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B10" r:id="rId92" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B9" r:id="rId93" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B8" r:id="rId94" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B7" r:id="rId95" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B6" r:id="rId96" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B5" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B4" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B3" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B2" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>